<commit_message>
update all features at thanh vien admin page
</commit_message>
<xml_diff>
--- a/src/main/resources/static/excel/thanhvien.xlsx
+++ b/src/main/resources/static/excel/thanhvien.xlsx
@@ -4,17 +4,30 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12210"/>
+    <workbookView windowWidth="27945" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>MaTV</t>
   </si>
@@ -43,7 +56,7 @@
     <t>CNTT</t>
   </si>
   <si>
-    <t>KTPM</t>
+    <t>Công nghệ phần mềm</t>
   </si>
   <si>
     <t>a@gmail.com</t>
@@ -52,19 +65,16 @@
     <t>Trần Thị B</t>
   </si>
   <si>
-    <t>ATTT</t>
-  </si>
-  <si>
     <t>b@gmail.com</t>
   </si>
   <si>
     <t>Le Van C</t>
   </si>
   <si>
-    <t>KT</t>
-  </si>
-  <si>
-    <t>Marketing</t>
+    <t>GDMN</t>
+  </si>
+  <si>
+    <t>Ngành giáo dục mầm non</t>
   </si>
   <si>
     <t>c@gmail.com</t>
@@ -79,7 +89,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -1235,7 +1245,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="6"/>
@@ -1243,7 +1253,7 @@
     <col min="1" max="1" width="11.8571428571429" customWidth="1"/>
     <col min="2" max="2" width="14.4285714285714" customWidth="1"/>
     <col min="3" max="3" width="6.14285714285714" customWidth="1"/>
-    <col min="4" max="4" width="10.5714285714286" customWidth="1"/>
+    <col min="4" max="4" width="39.1428571428571" customWidth="1"/>
     <col min="5" max="5" width="11.7142857142857" customWidth="1"/>
     <col min="6" max="6" width="13.2190476190476" customWidth="1"/>
     <col min="7" max="7" width="9.44761904761905" customWidth="1"/>
@@ -1306,13 +1316,13 @@
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E3" s="1">
         <v>1231231231</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G3" s="1">
         <v>123</v>
@@ -1323,19 +1333,19 @@
         <v>1124123458</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="E4" s="1">
         <v>2344322342</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" s="1">
         <v>123</v>
@@ -1352,13 +1362,13 @@
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1">
         <v>1231231231</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5" s="1">
         <v>123</v>
@@ -1369,19 +1379,19 @@
         <v>1199999999</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="E6" s="1">
         <v>111199999</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6" s="1">
         <v>123</v>
@@ -1392,19 +1402,19 @@
         <v>9999999999</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="E7" s="1">
         <v>199999999</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G7" s="1">
         <v>123</v>

</xml_diff>